<commit_message>
Deprecate upload-orange-metadata in favour of: - upload-metadata - upload-metadata-unique
</commit_message>
<xml_diff>
--- a/resolwe_bio/tests/files/metadata_upload/inputs/sample_metatable.xlsx
+++ b/resolwe_bio/tests/files/metadata_upload/inputs/sample_metatable.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janez/genialis/resolwe-bio/resolwe_bio/tests/files/metadata_upload/inputs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA04049-235D-EC41-89A0-541E09A66984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="11740" windowWidth="13920" windowHeight="8480" tabRatio="500"/>
+    <workbookView xWindow="7240" yWindow="11420" windowWidth="13920" windowHeight="8480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Untitled.tab" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Proteas</t>
   </si>
@@ -60,25 +66,52 @@
     <t>spo-mid</t>
   </si>
   <si>
-    <t>mD#function</t>
-  </si>
-  <si>
-    <t>mS#gene</t>
-  </si>
-  <si>
-    <t>c#heat 0</t>
-  </si>
-  <si>
-    <t>i#heat 10</t>
-  </si>
-  <si>
-    <t>i#heat 20</t>
+    <t>sample-1</t>
+  </si>
+  <si>
+    <t>sample-2</t>
+  </si>
+  <si>
+    <t>sample-3</t>
+  </si>
+  <si>
+    <t>sample-4</t>
+  </si>
+  <si>
+    <t>sample-5</t>
+  </si>
+  <si>
+    <t>sample-6</t>
+  </si>
+  <si>
+    <t>sample-7</t>
+  </si>
+  <si>
+    <t>sample-8</t>
+  </si>
+  <si>
+    <t>Sample slug</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>heat 0</t>
+  </si>
+  <si>
+    <t>heat 10</t>
+  </si>
+  <si>
+    <t>heat 20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -116,6 +149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -440,207 +481,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="G2">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="H2">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F3">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>-3.9E-2</v>
+      </c>
+      <c r="H3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="E4">
+        <v>-0.219</v>
+      </c>
+      <c r="F4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H4">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>-8.5000000000000006E-2</v>
+      </c>
+      <c r="E5">
+        <v>-0.161</v>
+      </c>
+      <c r="F5">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="G5">
+        <v>-0.26500000000000001</v>
+      </c>
+      <c r="H5">
+        <v>-0.41899999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="D2">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="F2">
-        <v>-8.9999999999999993E-3</v>
-      </c>
-      <c r="G2">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="E3">
-        <v>-6.0999999999999999E-2</v>
-      </c>
-      <c r="F3">
-        <v>-3.9E-2</v>
-      </c>
-      <c r="G3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>-0.216</v>
+      </c>
+      <c r="E6">
+        <v>-0.253</v>
+      </c>
+      <c r="F6">
+        <v>-0.22800000000000001</v>
+      </c>
+      <c r="G6">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="H6">
+        <v>-0.22800000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>-0.17899999999999999</v>
-      </c>
-      <c r="D4">
-        <v>-0.219</v>
-      </c>
-      <c r="E4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="G4">
-        <v>-1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>-8.5000000000000006E-2</v>
-      </c>
-      <c r="D5">
-        <v>-0.161</v>
-      </c>
-      <c r="E5">
-        <v>-6.0999999999999999E-2</v>
-      </c>
-      <c r="F5">
-        <v>-0.26500000000000001</v>
-      </c>
-      <c r="G5">
-        <v>-0.41899999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>-0.216</v>
-      </c>
-      <c r="D6">
-        <v>-0.253</v>
-      </c>
-      <c r="E6">
-        <v>-0.22800000000000001</v>
-      </c>
-      <c r="F6">
-        <v>-0.16800000000000001</v>
-      </c>
-      <c r="G6">
-        <v>-0.22800000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="H7">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="D7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E7">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="G7">
-        <v>0.20499999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>0.115</v>
+      </c>
+      <c r="F8">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="H8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>0.115</v>
-      </c>
-      <c r="E8">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F8">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="G8">
-        <v>5.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>-2.3E-2</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.222</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>8.7999999999999995E-2</v>
       </c>
     </row>

</xml_diff>